<commit_message>
Updated Version for Predictive Maintainance Template
</commit_message>
<xml_diff>
--- a/_templates/Predictive-Maintainance-Board/Sensor_Data_Barriers.xlsx
+++ b/_templates/Predictive-Maintainance-Board/Sensor_Data_Barriers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/git/peakboard-templates/_templates/Predictive-Maintainance-Board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCB8BFA-E1E1-8D4A-9A6D-91B5FA01182B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4135CA-B331-3140-9821-D2C2071D6E98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-54300" yWindow="-4160" windowWidth="42280" windowHeight="28600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,54 +23,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
-  <si>
-    <t>Engine1_Max</t>
-  </si>
-  <si>
-    <t>Engine2_Max</t>
-  </si>
-  <si>
-    <t>Temperature1_Max</t>
-  </si>
-  <si>
-    <t>Temperature2_Max</t>
-  </si>
-  <si>
-    <t>Temperature3_Max</t>
-  </si>
-  <si>
-    <t>ValveFlow1_Max</t>
-  </si>
-  <si>
-    <t>ValveFlow2_Max</t>
-  </si>
-  <si>
-    <t>Engine1_Min</t>
-  </si>
-  <si>
-    <t>Engine2_Min</t>
-  </si>
-  <si>
-    <t>Temperature1_Min</t>
-  </si>
-  <si>
-    <t>Temperature2_Min</t>
-  </si>
-  <si>
-    <t>Temperature3_Min</t>
-  </si>
-  <si>
-    <t>ValveFlow1_Min</t>
-  </si>
-  <si>
-    <t>ValveFlow2_Min</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>0.5</t>
   </si>
   <si>
     <t>0.004</t>
+  </si>
+  <si>
+    <t>Value1_Max</t>
+  </si>
+  <si>
+    <t>Value2_Max</t>
+  </si>
+  <si>
+    <t>Value3_Max</t>
+  </si>
+  <si>
+    <t>Value4_Max</t>
+  </si>
+  <si>
+    <t>Value5_Max</t>
+  </si>
+  <si>
+    <t>Value6_Max</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Value7_Max</t>
+  </si>
+  <si>
+    <t>Value1_Warning</t>
+  </si>
+  <si>
+    <t>Value2_Warning</t>
+  </si>
+  <si>
+    <t>Value3_Warning</t>
+  </si>
+  <si>
+    <t>Value4_Warning</t>
+  </si>
+  <si>
+    <t>Value5_Warning</t>
+  </si>
+  <si>
+    <t>Value6_Warning</t>
+  </si>
+  <si>
+    <t>Value7_Warning</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.002</t>
   </si>
 </sst>
 </file>
@@ -429,7 +435,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -442,54 +448,54 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
         <v>80</v>
@@ -501,31 +507,31 @@
         <v>80</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="J2" s="1">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="K2" s="1">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="L2" s="1">
-        <v>40</v>
-      </c>
-      <c r="M2" s="1">
-        <v>0</v>
-      </c>
-      <c r="N2" s="1">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>